<commit_message>
update car, lunch, car ratings and lunch ratings models
</commit_message>
<xml_diff>
--- a/Examples/AHP_Lunch/lunchModel_Results.xlsx
+++ b/Examples/AHP_Lunch/lunchModel_Results.xlsx
@@ -8,15 +8,16 @@
   </bookViews>
   <sheets>
     <sheet name="pairwise_comp" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="supermatrix" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="limit matrix" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="limitingPriorities" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="localPriorities" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Sens_1Quality" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Sens_2Price" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Sens_3Menu" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Sens_4Speed" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Graph Model" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Graph Model" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="supermatrix" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="limit matrix" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="limitingPriorities" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="localPriorities" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Sens_1Quality" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Sens_2Price" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Sens_3Menu" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Sens_4Speed" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="Graph Model1" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -898,7 +899,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -1945,7 +1946,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1968,366 +1968,41 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="15" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
-    <col width="15" customWidth="1" min="3" max="3"/>
-    <col width="15" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" min="5" max="5"/>
-    <col width="15" customWidth="1" min="6" max="6"/>
-    <col width="15" customWidth="1" min="7" max="7"/>
-    <col width="15" customWidth="1" min="8" max="8"/>
-    <col width="15" customWidth="1" min="9" max="9"/>
-    <col width="15" customWidth="1" min="10" max="10"/>
-  </cols>
-  <sheetData>
-    <row r="1">
-      <c r="C1" s="26" t="inlineStr">
-        <is>
-          <t>1Goal</t>
-        </is>
-      </c>
-      <c r="D1" s="26" t="inlineStr">
-        <is>
-          <t>2Criteria</t>
-        </is>
-      </c>
-      <c r="E1" s="27" t="inlineStr"/>
-      <c r="F1" s="27" t="inlineStr"/>
-      <c r="G1" s="27" t="inlineStr"/>
-      <c r="H1" s="26" t="inlineStr">
-        <is>
-          <t>3Alternatives</t>
-        </is>
-      </c>
-      <c r="I1" s="27" t="inlineStr"/>
-      <c r="J1" s="27" t="inlineStr"/>
-    </row>
-    <row r="2">
-      <c r="C2" s="25" t="inlineStr">
-        <is>
-          <t>GoalNode</t>
-        </is>
-      </c>
-      <c r="D2" s="25" t="inlineStr">
-        <is>
-          <t>1Quality</t>
-        </is>
-      </c>
-      <c r="E2" s="25" t="inlineStr">
-        <is>
-          <t>2Price</t>
-        </is>
-      </c>
-      <c r="F2" s="25" t="inlineStr">
-        <is>
-          <t>3Menu</t>
-        </is>
-      </c>
-      <c r="G2" s="25" t="inlineStr">
-        <is>
-          <t>4Speed</t>
-        </is>
-      </c>
-      <c r="H2" s="25" t="inlineStr">
-        <is>
-          <t>1Primanti</t>
-        </is>
-      </c>
-      <c r="I2" s="25" t="inlineStr">
-        <is>
-          <t>2Panera</t>
-        </is>
-      </c>
-      <c r="J2" s="25" t="inlineStr">
-        <is>
-          <t>3Piada</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="26" t="inlineStr">
-        <is>
-          <t>1Goal</t>
-        </is>
-      </c>
-      <c r="B3" s="25" t="inlineStr">
-        <is>
-          <t>GoalNode</t>
-        </is>
-      </c>
-      <c r="C3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="26" t="inlineStr">
-        <is>
-          <t>2Criteria</t>
-        </is>
-      </c>
-      <c r="B4" s="25" t="inlineStr">
-        <is>
-          <t>1Quality</t>
-        </is>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>0.379</v>
-      </c>
-      <c r="D4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="27" t="inlineStr"/>
-      <c r="B5" s="25" t="inlineStr">
-        <is>
-          <t>2Price</t>
-        </is>
-      </c>
-      <c r="C5" s="7" t="n">
-        <v>0.189</v>
-      </c>
-      <c r="D5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="27" t="inlineStr"/>
-      <c r="B6" s="25" t="inlineStr">
-        <is>
-          <t>3Menu</t>
-        </is>
-      </c>
-      <c r="C6" s="7" t="n">
-        <v>0.217</v>
-      </c>
-      <c r="D6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="27" t="inlineStr"/>
-      <c r="B7" s="25" t="inlineStr">
-        <is>
-          <t>4Speed</t>
-        </is>
-      </c>
-      <c r="C7" s="7" t="n">
-        <v>0.215</v>
-      </c>
-      <c r="D7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="G7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="H7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I7" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="26" t="inlineStr">
-        <is>
-          <t>3Alternatives</t>
-        </is>
-      </c>
-      <c r="B8" s="25" t="inlineStr">
-        <is>
-          <t>1Primanti</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="7" t="n">
-        <v>0.168</v>
-      </c>
-      <c r="E8" s="7" t="n">
-        <v>0.381</v>
-      </c>
-      <c r="F8" s="7" t="n">
-        <v>0.096</v>
-      </c>
-      <c r="G8" s="7" t="n">
-        <v>0.55</v>
-      </c>
-      <c r="H8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I8" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="27" t="inlineStr"/>
-      <c r="B9" s="25" t="inlineStr">
-        <is>
-          <t>2Panera</t>
-        </is>
-      </c>
-      <c r="C9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="7" t="n">
-        <v>0.484</v>
-      </c>
-      <c r="E9" s="7" t="n">
-        <v>0.347</v>
-      </c>
-      <c r="F9" s="7" t="n">
-        <v>0.596</v>
-      </c>
-      <c r="G9" s="7" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="H9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="27" t="inlineStr"/>
-      <c r="B10" s="25" t="inlineStr">
-        <is>
-          <t>3Piada</t>
-        </is>
-      </c>
-      <c r="C10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" s="7" t="n">
-        <v>0.349</v>
-      </c>
-      <c r="E10" s="7" t="n">
-        <v>0.272</v>
-      </c>
-      <c r="F10" s="7" t="n">
-        <v>0.308</v>
-      </c>
-      <c r="G10" s="7" t="n">
-        <v>0.24</v>
-      </c>
-      <c r="H10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="7" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="7" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2469,7 +2144,7 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>0.189</v>
+        <v>0.379</v>
       </c>
       <c r="D4" s="7" t="n">
         <v>0</v>
@@ -2501,7 +2176,7 @@
         </is>
       </c>
       <c r="C5" s="7" t="n">
-        <v>0.095</v>
+        <v>0.189</v>
       </c>
       <c r="D5" s="7" t="n">
         <v>0</v>
@@ -2533,7 +2208,7 @@
         </is>
       </c>
       <c r="C6" s="7" t="n">
-        <v>0.108</v>
+        <v>0.217</v>
       </c>
       <c r="D6" s="7" t="n">
         <v>0</v>
@@ -2565,7 +2240,7 @@
         </is>
       </c>
       <c r="C7" s="7" t="n">
-        <v>0.108</v>
+        <v>0.215</v>
       </c>
       <c r="D7" s="7" t="n">
         <v>0</v>
@@ -2601,7 +2276,7 @@
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>0.137</v>
+        <v>0</v>
       </c>
       <c r="D8" s="7" t="n">
         <v>0.168</v>
@@ -2633,7 +2308,7 @@
         </is>
       </c>
       <c r="C9" s="7" t="n">
-        <v>0.211</v>
+        <v>0</v>
       </c>
       <c r="D9" s="7" t="n">
         <v>0.484</v>
@@ -2665,7 +2340,7 @@
         </is>
       </c>
       <c r="C10" s="7" t="n">
-        <v>0.151</v>
+        <v>0</v>
       </c>
       <c r="D10" s="7" t="n">
         <v>0.349</v>
@@ -2700,7 +2375,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2711,113 +2386,345 @@
     <col width="15" customWidth="1" min="1" max="1"/>
     <col width="15" customWidth="1" min="2" max="2"/>
     <col width="15" customWidth="1" min="3" max="3"/>
+    <col width="15" customWidth="1" min="4" max="4"/>
+    <col width="15" customWidth="1" min="5" max="5"/>
+    <col width="15" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
+    <col width="15" customWidth="1" min="8" max="8"/>
+    <col width="15" customWidth="1" min="9" max="9"/>
+    <col width="15" customWidth="1" min="10" max="10"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="C1" s="25" t="inlineStr">
-        <is>
-          <t>Limiting Prior.</t>
-        </is>
-      </c>
+      <c r="C1" s="26" t="inlineStr">
+        <is>
+          <t>1Goal</t>
+        </is>
+      </c>
+      <c r="D1" s="26" t="inlineStr">
+        <is>
+          <t>2Criteria</t>
+        </is>
+      </c>
+      <c r="E1" s="27" t="inlineStr"/>
+      <c r="F1" s="27" t="inlineStr"/>
+      <c r="G1" s="27" t="inlineStr"/>
+      <c r="H1" s="26" t="inlineStr">
+        <is>
+          <t>3Alternatives</t>
+        </is>
+      </c>
+      <c r="I1" s="27" t="inlineStr"/>
+      <c r="J1" s="27" t="inlineStr"/>
     </row>
     <row r="2">
-      <c r="A2" s="26" t="inlineStr">
-        <is>
-          <t>1Goal</t>
-        </is>
-      </c>
-      <c r="B2" s="25" t="inlineStr">
+      <c r="C2" s="25" t="inlineStr">
         <is>
           <t>GoalNode</t>
         </is>
       </c>
-      <c r="C2" s="7" t="n">
-        <v>0</v>
+      <c r="D2" s="25" t="inlineStr">
+        <is>
+          <t>1Quality</t>
+        </is>
+      </c>
+      <c r="E2" s="25" t="inlineStr">
+        <is>
+          <t>2Price</t>
+        </is>
+      </c>
+      <c r="F2" s="25" t="inlineStr">
+        <is>
+          <t>3Menu</t>
+        </is>
+      </c>
+      <c r="G2" s="25" t="inlineStr">
+        <is>
+          <t>4Speed</t>
+        </is>
+      </c>
+      <c r="H2" s="25" t="inlineStr">
+        <is>
+          <t>1Primanti</t>
+        </is>
+      </c>
+      <c r="I2" s="25" t="inlineStr">
+        <is>
+          <t>2Panera</t>
+        </is>
+      </c>
+      <c r="J2" s="25" t="inlineStr">
+        <is>
+          <t>3Piada</t>
+        </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="26" t="inlineStr">
         <is>
+          <t>1Goal</t>
+        </is>
+      </c>
+      <c r="B3" s="25" t="inlineStr">
+        <is>
+          <t>GoalNode</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="26" t="inlineStr">
+        <is>
           <t>2Criteria</t>
         </is>
       </c>
-      <c r="B3" s="25" t="inlineStr">
+      <c r="B4" s="25" t="inlineStr">
         <is>
           <t>1Quality</t>
         </is>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C4" s="7" t="n">
         <v>0.189</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="27" t="inlineStr"/>
-      <c r="B4" s="25" t="inlineStr">
-        <is>
-          <t>2Price</t>
-        </is>
-      </c>
-      <c r="C4" s="7" t="n">
-        <v>0.095</v>
+      <c r="D4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="27" t="inlineStr"/>
       <c r="B5" s="25" t="inlineStr">
         <is>
-          <t>3Menu</t>
+          <t>2Price</t>
         </is>
       </c>
       <c r="C5" s="7" t="n">
-        <v>0.108</v>
+        <v>0.095</v>
+      </c>
+      <c r="D5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="27" t="inlineStr"/>
       <c r="B6" s="25" t="inlineStr">
         <is>
-          <t>4Speed</t>
+          <t>3Menu</t>
         </is>
       </c>
       <c r="C6" s="7" t="n">
         <v>0.108</v>
       </c>
+      <c r="D6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="26" t="inlineStr">
+      <c r="A7" s="27" t="inlineStr"/>
+      <c r="B7" s="25" t="inlineStr">
+        <is>
+          <t>4Speed</t>
+        </is>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="D7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="26" t="inlineStr">
         <is>
           <t>3Alternatives</t>
         </is>
       </c>
-      <c r="B7" s="25" t="inlineStr">
+      <c r="B8" s="25" t="inlineStr">
         <is>
           <t>1Primanti</t>
         </is>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C8" s="7" t="n">
         <v>0.137</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="27" t="inlineStr"/>
-      <c r="B8" s="25" t="inlineStr">
-        <is>
-          <t>2Panera</t>
-        </is>
-      </c>
-      <c r="C8" s="7" t="n">
-        <v>0.211</v>
+      <c r="D8" s="7" t="n">
+        <v>0.168</v>
+      </c>
+      <c r="E8" s="7" t="n">
+        <v>0.381</v>
+      </c>
+      <c r="F8" s="7" t="n">
+        <v>0.096</v>
+      </c>
+      <c r="G8" s="7" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="27" t="inlineStr"/>
       <c r="B9" s="25" t="inlineStr">
         <is>
+          <t>2Panera</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.211</v>
+      </c>
+      <c r="D9" s="7" t="n">
+        <v>0.484</v>
+      </c>
+      <c r="E9" s="7" t="n">
+        <v>0.347</v>
+      </c>
+      <c r="F9" s="7" t="n">
+        <v>0.596</v>
+      </c>
+      <c r="G9" s="7" t="n">
+        <v>0.21</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="27" t="inlineStr"/>
+      <c r="B10" s="25" t="inlineStr">
+        <is>
           <t>3Piada</t>
         </is>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C10" s="7" t="n">
         <v>0.151</v>
+      </c>
+      <c r="D10" s="7" t="n">
+        <v>0.349</v>
+      </c>
+      <c r="E10" s="7" t="n">
+        <v>0.272</v>
+      </c>
+      <c r="F10" s="7" t="n">
+        <v>0.308</v>
+      </c>
+      <c r="G10" s="7" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2847,7 +2754,7 @@
     <row r="1">
       <c r="C1" s="25" t="inlineStr">
         <is>
-          <t>Local Priorities</t>
+          <t>Limiting Prior.</t>
         </is>
       </c>
     </row>
@@ -2878,7 +2785,7 @@
         </is>
       </c>
       <c r="C3" s="7" t="n">
-        <v>0.379</v>
+        <v>0.189</v>
       </c>
     </row>
     <row r="4">
@@ -2889,7 +2796,7 @@
         </is>
       </c>
       <c r="C4" s="7" t="n">
-        <v>0.189</v>
+        <v>0.095</v>
       </c>
     </row>
     <row r="5">
@@ -2900,7 +2807,7 @@
         </is>
       </c>
       <c r="C5" s="7" t="n">
-        <v>0.217</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="6">
@@ -2911,7 +2818,7 @@
         </is>
       </c>
       <c r="C6" s="7" t="n">
-        <v>0.215</v>
+        <v>0.108</v>
       </c>
     </row>
     <row r="7">
@@ -2926,7 +2833,7 @@
         </is>
       </c>
       <c r="C7" s="7" t="n">
-        <v>0.275</v>
+        <v>0.137</v>
       </c>
     </row>
     <row r="8">
@@ -2937,7 +2844,7 @@
         </is>
       </c>
       <c r="C8" s="7" t="n">
-        <v>0.423</v>
+        <v>0.211</v>
       </c>
     </row>
     <row r="9">
@@ -2948,7 +2855,7 @@
         </is>
       </c>
       <c r="C9" s="7" t="n">
-        <v>0.302</v>
+        <v>0.151</v>
       </c>
     </row>
   </sheetData>
@@ -2957,21 +2864,133 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col width="15" customWidth="1" min="1" max="1"/>
+    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="15" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="C1" s="25" t="inlineStr">
+        <is>
+          <t>Local Priorities</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="26" t="inlineStr">
+        <is>
+          <t>1Goal</t>
+        </is>
+      </c>
+      <c r="B2" s="25" t="inlineStr">
+        <is>
+          <t>GoalNode</t>
+        </is>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="26" t="inlineStr">
+        <is>
+          <t>2Criteria</t>
+        </is>
+      </c>
+      <c r="B3" s="25" t="inlineStr">
+        <is>
+          <t>1Quality</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>0.379</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="27" t="inlineStr"/>
+      <c r="B4" s="25" t="inlineStr">
+        <is>
+          <t>2Price</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="27" t="inlineStr"/>
+      <c r="B5" s="25" t="inlineStr">
+        <is>
+          <t>3Menu</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>0.217</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="27" t="inlineStr"/>
+      <c r="B6" s="25" t="inlineStr">
+        <is>
+          <t>4Speed</t>
+        </is>
+      </c>
+      <c r="C6" s="7" t="n">
+        <v>0.215</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="26" t="inlineStr">
+        <is>
+          <t>3Alternatives</t>
+        </is>
+      </c>
+      <c r="B7" s="25" t="inlineStr">
+        <is>
+          <t>1Primanti</t>
+        </is>
+      </c>
+      <c r="C7" s="7" t="n">
+        <v>0.275</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="27" t="inlineStr"/>
+      <c r="B8" s="25" t="inlineStr">
+        <is>
+          <t>2Panera</t>
+        </is>
+      </c>
+      <c r="C8" s="7" t="n">
+        <v>0.423</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="27" t="inlineStr"/>
+      <c r="B9" s="25" t="inlineStr">
+        <is>
+          <t>3Piada</t>
+        </is>
+      </c>
+      <c r="C9" s="7" t="n">
+        <v>0.302</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>